<commit_message>
Add ranking column and improve prediction logic (max 1000 points)
</commit_message>
<xml_diff>
--- a/data/latest_data.xlsx
+++ b/data/latest_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD54C82D-3ED5-426D-9413-F19197FFAF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEA01C6-3670-4158-8CD1-8BCECA660ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{374363BE-A5F5-4ADC-8A41-9D43B010FE25}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>센터명</t>
   </si>
@@ -141,6 +141,10 @@
   </si>
   <si>
     <t>별내</t>
+  </si>
+  <si>
+    <t>총점</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -252,7 +256,7 @@
     <xf numFmtId="17" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -590,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576B49EF-D72C-489F-81B1-8DBFDE47B864}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -601,7 +605,7 @@
     <col min="1" max="11" width="20.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -635,8 +639,11 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -659,7 +666,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="2">
-        <v>89</v>
+        <v>95.365000000000009</v>
       </c>
       <c r="I2" s="2">
         <v>0</v>
@@ -670,8 +677,11 @@
       <c r="K2" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L2">
+        <v>463.80709747340745</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -694,7 +704,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="2">
-        <v>92</v>
+        <v>94.01333333333335</v>
       </c>
       <c r="I3" s="2">
         <v>0</v>
@@ -705,8 +715,11 @@
       <c r="K3" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L3">
+        <v>509.779255735893</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -729,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="2">
-        <v>90</v>
+        <v>94.268666666666675</v>
       </c>
       <c r="I4" s="2">
         <v>0</v>
@@ -740,8 +753,11 @@
       <c r="K4" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L4">
+        <v>508.43764615948845</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -764,7 +780,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="2">
-        <v>88</v>
+        <v>92.329333333333338</v>
       </c>
       <c r="I5" s="2">
         <v>0</v>
@@ -775,8 +791,11 @@
       <c r="K5" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L5">
+        <v>551.58837853897785</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -799,7 +818,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="2">
-        <v>85</v>
+        <v>96.663333333333327</v>
       </c>
       <c r="I6" s="2">
         <v>0</v>
@@ -810,8 +829,11 @@
       <c r="K6" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L6">
+        <v>514.80953003884827</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -834,7 +856,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="2">
-        <v>93</v>
+        <v>91.872450980392145</v>
       </c>
       <c r="I7" s="2">
         <v>0</v>
@@ -845,8 +867,11 @@
       <c r="K7" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L7">
+        <v>532.64897714174049</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -869,7 +894,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="2">
-        <v>87</v>
+        <v>91.523333333333355</v>
       </c>
       <c r="I8" s="2">
         <v>0</v>
@@ -880,8 +905,11 @@
       <c r="K8" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L8">
+        <v>523.4641558791443</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -904,7 +932,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="2">
-        <v>91</v>
+        <v>91.427916666666675</v>
       </c>
       <c r="I9" s="2">
         <v>0</v>
@@ -915,8 +943,11 @@
       <c r="K9" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L9">
+        <v>482.35872777761529</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -939,7 +970,7 @@
         <v>0.95479359567901234</v>
       </c>
       <c r="H10" s="2">
-        <v>86</v>
+        <v>92.385800000000003</v>
       </c>
       <c r="I10" s="2">
         <v>0</v>
@@ -950,8 +981,11 @@
       <c r="K10" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L10">
+        <v>439.37030476884786</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -974,7 +1008,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="2">
-        <v>89</v>
+        <v>94.566666666666677</v>
       </c>
       <c r="I11" s="2">
         <v>0</v>
@@ -985,8 +1019,11 @@
       <c r="K11" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L11">
+        <v>516.92437748568875</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -1009,7 +1046,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="2">
-        <v>87</v>
+        <v>93.165294117647065</v>
       </c>
       <c r="I12" s="2">
         <v>0</v>
@@ -1020,8 +1057,11 @@
       <c r="K12" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L12">
+        <v>509.64134279991544</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -1044,7 +1084,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="2">
-        <v>88</v>
+        <v>92.768965517241355</v>
       </c>
       <c r="I13" s="2">
         <v>0</v>
@@ -1055,8 +1095,11 @@
       <c r="K13" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L13">
+        <v>530.58480932894827</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -1079,7 +1122,7 @@
         <v>1</v>
       </c>
       <c r="H14" s="2">
-        <v>86</v>
+        <v>93.998620689655169</v>
       </c>
       <c r="I14" s="2">
         <v>0</v>
@@ -1090,8 +1133,11 @@
       <c r="K14" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L14">
+        <v>459.45930791816983</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
@@ -1114,7 +1160,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="2">
-        <v>90</v>
+        <v>95.604000000000013</v>
       </c>
       <c r="I15" s="2">
         <v>0</v>
@@ -1125,8 +1171,11 @@
       <c r="K15" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L15">
+        <v>533.21314653384434</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
@@ -1149,7 +1198,7 @@
         <v>1</v>
       </c>
       <c r="H16" s="2">
-        <v>89</v>
+        <v>93.432857142857159</v>
       </c>
       <c r="I16" s="2">
         <v>0</v>
@@ -1160,8 +1209,11 @@
       <c r="K16" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L16">
+        <v>513.67975035674112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -1184,7 +1236,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="2">
-        <v>91</v>
+        <v>93.817777777777778</v>
       </c>
       <c r="I17" s="2">
         <v>0</v>
@@ -1195,8 +1247,11 @@
       <c r="K17" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L17">
+        <v>483.252629632631</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
@@ -1219,7 +1274,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="2">
-        <v>88</v>
+        <v>93.785054945054938</v>
       </c>
       <c r="I18" s="2">
         <v>0</v>
@@ -1230,8 +1285,11 @@
       <c r="K18" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L18">
+        <v>477.33895611897816</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>28</v>
       </c>
@@ -1254,7 +1312,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="2">
-        <v>90</v>
+        <v>95.439523809523834</v>
       </c>
       <c r="I19" s="2">
         <v>0</v>
@@ -1265,8 +1323,11 @@
       <c r="K19" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L19">
+        <v>534.4577540769003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>29</v>
       </c>
@@ -1289,7 +1350,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="2">
-        <v>86</v>
+        <v>94.19380392156863</v>
       </c>
       <c r="I20" s="2">
         <v>0</v>
@@ -1300,8 +1361,11 @@
       <c r="K20" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L20">
+        <v>497.7841767466939</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
@@ -1324,7 +1388,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="2">
-        <v>87</v>
+        <v>93.901714285714291</v>
       </c>
       <c r="I21" s="2">
         <v>0</v>
@@ -1335,8 +1399,11 @@
       <c r="K21" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L21">
+        <v>476.23547691598753</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>31</v>
       </c>
@@ -1359,7 +1426,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="2">
-        <v>94</v>
+        <v>93.098181818181843</v>
       </c>
       <c r="I22" s="2">
         <v>0</v>
@@ -1370,8 +1437,11 @@
       <c r="K22" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L22">
+        <v>586.24680398898033</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>32</v>
       </c>
@@ -1394,7 +1464,7 @@
         <v>1</v>
       </c>
       <c r="H23" s="2">
-        <v>88</v>
+        <v>94.451264367816108</v>
       </c>
       <c r="I23" s="2">
         <v>0</v>
@@ -1405,8 +1475,11 @@
       <c r="K23" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L23">
+        <v>501.21121229136116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>33</v>
       </c>
@@ -1429,7 +1502,7 @@
         <v>1</v>
       </c>
       <c r="H24" s="2">
-        <v>85</v>
+        <v>92.290476190476213</v>
       </c>
       <c r="I24" s="2">
         <v>0</v>
@@ -1440,8 +1513,11 @@
       <c r="K24" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L24">
+        <v>496.72199126218618</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>34</v>
       </c>
@@ -1464,7 +1540,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="2">
-        <v>92</v>
+        <v>93.188260869565227</v>
       </c>
       <c r="I25" s="2">
         <v>0</v>
@@ -1474,6 +1550,9 @@
       </c>
       <c r="K25" s="2">
         <v>0</v>
+      </c>
+      <c r="L25">
+        <v>500.04382922399441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>